<commit_message>
finish the last step
</commit_message>
<xml_diff>
--- a/example/result.xlsx
+++ b/example/result.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Yingheng\Project\Elastic_MBQC\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49609EAB-D990-4F38-9DA7-DBFCA2410D29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D67A86A-AA57-43DD-85A0-7EF5406F4A7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="5" sheetId="4" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="75">
   <si>
     <t>Bench</t>
   </si>
@@ -240,6 +240,30 @@
   </si>
   <si>
     <t>hlf7(21)</t>
+  </si>
+  <si>
+    <t>hlf10(19)</t>
+  </si>
+  <si>
+    <t>hlf10(26)</t>
+  </si>
+  <si>
+    <t>hlf10(21)</t>
+  </si>
+  <si>
+    <t>hlf10(24)</t>
+  </si>
+  <si>
+    <t>hlf12(26)</t>
+  </si>
+  <si>
+    <t>hlf12(23)</t>
+  </si>
+  <si>
+    <t>hlf12(34)</t>
+  </si>
+  <si>
+    <t>hlf12(30)</t>
   </si>
 </sst>
 </file>
@@ -566,7 +590,7 @@
   <dimension ref="A1:U17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="T14" sqref="T14"/>
+      <selection activeCell="M14" sqref="M14:M17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1635,10 +1659,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U13"/>
+  <dimension ref="A1:U17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T6" sqref="T6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M14" sqref="M14:U17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1844,15 +1868,15 @@
         <v>35</v>
       </c>
       <c r="S3">
-        <f t="shared" ref="S3:S13" si="4">(O3-Q3)/N3</f>
+        <f t="shared" ref="S3:S17" si="4">(O3-Q3)/N3</f>
         <v>0.19642857142857142</v>
       </c>
       <c r="T3">
-        <f t="shared" ref="T3:T13" si="5">(P3-R3+Q3)/N3</f>
+        <f t="shared" ref="T3:T17" si="5">(P3-R3+Q3)/N3</f>
         <v>0.17857142857142858</v>
       </c>
       <c r="U3">
-        <f t="shared" ref="U3:U13" si="6" xml:space="preserve"> 1 -R3/N3</f>
+        <f t="shared" ref="U3:U17" si="6" xml:space="preserve"> 1 -R3/N3</f>
         <v>0.375</v>
       </c>
     </row>
@@ -2118,7 +2142,7 @@
         <v>48</v>
       </c>
       <c r="P7">
-        <f t="shared" ref="P7:P13" si="8">N7-O7</f>
+        <f t="shared" ref="P7:P17" si="8">N7-O7</f>
         <v>8</v>
       </c>
       <c r="Q7">
@@ -2564,6 +2588,138 @@
       <c r="U13">
         <f t="shared" si="6"/>
         <v>5.0000000000000044E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="M14" t="s">
+        <v>68</v>
+      </c>
+      <c r="N14">
+        <v>28</v>
+      </c>
+      <c r="O14">
+        <v>22</v>
+      </c>
+      <c r="P14">
+        <f t="shared" si="8"/>
+        <v>6</v>
+      </c>
+      <c r="Q14">
+        <v>16</v>
+      </c>
+      <c r="R14">
+        <v>19</v>
+      </c>
+      <c r="S14">
+        <f t="shared" si="4"/>
+        <v>0.21428571428571427</v>
+      </c>
+      <c r="T14">
+        <f t="shared" si="5"/>
+        <v>0.10714285714285714</v>
+      </c>
+      <c r="U14">
+        <f t="shared" si="6"/>
+        <v>0.3214285714285714</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="M15" t="s">
+        <v>70</v>
+      </c>
+      <c r="N15">
+        <v>28</v>
+      </c>
+      <c r="O15">
+        <v>22</v>
+      </c>
+      <c r="P15">
+        <f t="shared" si="8"/>
+        <v>6</v>
+      </c>
+      <c r="Q15">
+        <v>17</v>
+      </c>
+      <c r="R15">
+        <v>21</v>
+      </c>
+      <c r="S15">
+        <f t="shared" si="4"/>
+        <v>0.17857142857142858</v>
+      </c>
+      <c r="T15">
+        <f t="shared" si="5"/>
+        <v>7.1428571428571425E-2</v>
+      </c>
+      <c r="U15">
+        <f t="shared" si="6"/>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="M16" t="s">
+        <v>69</v>
+      </c>
+      <c r="N16">
+        <v>28</v>
+      </c>
+      <c r="O16">
+        <v>22</v>
+      </c>
+      <c r="P16">
+        <f t="shared" si="8"/>
+        <v>6</v>
+      </c>
+      <c r="Q16">
+        <v>20</v>
+      </c>
+      <c r="R16">
+        <v>23</v>
+      </c>
+      <c r="S16">
+        <f t="shared" si="4"/>
+        <v>7.1428571428571425E-2</v>
+      </c>
+      <c r="T16">
+        <f t="shared" si="5"/>
+        <v>0.10714285714285714</v>
+      </c>
+      <c r="U16">
+        <f t="shared" si="6"/>
+        <v>0.1785714285714286</v>
+      </c>
+    </row>
+    <row r="17" spans="13:21" x14ac:dyDescent="0.25">
+      <c r="M17" t="s">
+        <v>67</v>
+      </c>
+      <c r="N17">
+        <v>28</v>
+      </c>
+      <c r="O17">
+        <v>22</v>
+      </c>
+      <c r="P17">
+        <f t="shared" si="8"/>
+        <v>6</v>
+      </c>
+      <c r="Q17">
+        <v>22</v>
+      </c>
+      <c r="R17">
+        <v>25</v>
+      </c>
+      <c r="S17">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="T17">
+        <f t="shared" si="5"/>
+        <v>0.10714285714285714</v>
+      </c>
+      <c r="U17">
+        <f t="shared" si="6"/>
+        <v>0.1071428571428571</v>
       </c>
     </row>
   </sheetData>
@@ -2574,10 +2730,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4122154B-B607-4FC5-B72D-2D5F47AE10A5}">
-  <dimension ref="A1:U15"/>
+  <dimension ref="A1:U19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="T8" sqref="T8"/>
+      <selection activeCell="S12" sqref="S12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2781,15 +2937,15 @@
         <v>38</v>
       </c>
       <c r="S3">
-        <f t="shared" ref="S3:S15" si="5">(O3-Q3)/N3</f>
+        <f t="shared" ref="S3:S19" si="5">(O3-Q3)/N3</f>
         <v>0.29411764705882354</v>
       </c>
       <c r="T3">
-        <f t="shared" ref="T3:T15" si="6">(P3-R3+Q3)/N3</f>
+        <f t="shared" ref="T3:T19" si="6">(P3-R3+Q3)/N3</f>
         <v>0.14705882352941177</v>
       </c>
       <c r="U3">
-        <f t="shared" ref="U3:U15" si="7" xml:space="preserve"> 1 -R3/N3</f>
+        <f t="shared" ref="U3:U19" si="7" xml:space="preserve"> 1 -R3/N3</f>
         <v>0.44117647058823528</v>
       </c>
     </row>
@@ -3055,7 +3211,7 @@
         <v>55</v>
       </c>
       <c r="P7">
-        <f t="shared" ref="P7:P15" si="12">N7-O7</f>
+        <f t="shared" ref="P7:P19" si="12">N7-O7</f>
         <v>13</v>
       </c>
       <c r="Q7">
@@ -3643,6 +3799,138 @@
       <c r="U15">
         <f t="shared" si="7"/>
         <v>4.166666666666663E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="M16" t="s">
+        <v>73</v>
+      </c>
+      <c r="N16">
+        <v>40</v>
+      </c>
+      <c r="O16">
+        <v>34</v>
+      </c>
+      <c r="P16">
+        <f t="shared" si="12"/>
+        <v>6</v>
+      </c>
+      <c r="Q16">
+        <v>23</v>
+      </c>
+      <c r="R16">
+        <v>25</v>
+      </c>
+      <c r="S16">
+        <f t="shared" si="5"/>
+        <v>0.27500000000000002</v>
+      </c>
+      <c r="T16">
+        <f t="shared" si="6"/>
+        <v>0.1</v>
+      </c>
+      <c r="U16">
+        <f t="shared" si="7"/>
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="17" spans="13:21" x14ac:dyDescent="0.25">
+      <c r="M17" t="s">
+        <v>74</v>
+      </c>
+      <c r="N17">
+        <v>40</v>
+      </c>
+      <c r="O17">
+        <v>34</v>
+      </c>
+      <c r="P17">
+        <f t="shared" si="12"/>
+        <v>6</v>
+      </c>
+      <c r="Q17">
+        <v>25</v>
+      </c>
+      <c r="R17">
+        <v>29</v>
+      </c>
+      <c r="S17">
+        <f t="shared" si="5"/>
+        <v>0.22500000000000001</v>
+      </c>
+      <c r="T17">
+        <f t="shared" si="6"/>
+        <v>0.05</v>
+      </c>
+      <c r="U17">
+        <f t="shared" si="7"/>
+        <v>0.27500000000000002</v>
+      </c>
+    </row>
+    <row r="18" spans="13:21" x14ac:dyDescent="0.25">
+      <c r="M18" t="s">
+        <v>71</v>
+      </c>
+      <c r="N18">
+        <v>40</v>
+      </c>
+      <c r="O18">
+        <v>34</v>
+      </c>
+      <c r="P18">
+        <f t="shared" si="12"/>
+        <v>6</v>
+      </c>
+      <c r="Q18">
+        <v>28</v>
+      </c>
+      <c r="R18">
+        <v>31</v>
+      </c>
+      <c r="S18">
+        <f t="shared" si="5"/>
+        <v>0.15</v>
+      </c>
+      <c r="T18">
+        <f t="shared" si="6"/>
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="U18">
+        <f t="shared" si="7"/>
+        <v>0.22499999999999998</v>
+      </c>
+    </row>
+    <row r="19" spans="13:21" x14ac:dyDescent="0.25">
+      <c r="M19" t="s">
+        <v>72</v>
+      </c>
+      <c r="N19">
+        <v>40</v>
+      </c>
+      <c r="O19">
+        <v>34</v>
+      </c>
+      <c r="P19">
+        <f t="shared" si="12"/>
+        <v>6</v>
+      </c>
+      <c r="Q19">
+        <v>34</v>
+      </c>
+      <c r="R19">
+        <v>38</v>
+      </c>
+      <c r="S19">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="T19">
+        <f t="shared" si="6"/>
+        <v>0.05</v>
+      </c>
+      <c r="U19">
+        <f t="shared" si="7"/>
+        <v>5.0000000000000044E-2</v>
       </c>
     </row>
   </sheetData>
@@ -3654,7 +3942,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{295084A2-B2D2-4E5F-BB0C-D346381CD2B2}">
   <dimension ref="A1:I15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
finish the recording the combination
</commit_message>
<xml_diff>
--- a/example/result.xlsx
+++ b/example/result.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Yingheng\Project\Elastic_MBQC\example\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\pitt_research\Elastic_MBQC\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E30A05EA-A939-4580-B183-2F2E6D348ACE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F88375D-05F3-4749-A2CE-4099BAB84185}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="18465" yWindow="4395" windowWidth="27810" windowHeight="16635" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="5" sheetId="4" r:id="rId1"/>
@@ -1673,8 +1673,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M14" sqref="M14:U17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3954,7 +3954,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{295084A2-B2D2-4E5F-BB0C-D346381CD2B2}">
   <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
finish the last benchmarks
</commit_message>
<xml_diff>
--- a/example/result.xlsx
+++ b/example/result.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\pitt_research\Elastic_MBQC\example\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Yingheng\Project\Elastic_MBQC\example\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E406677-D0E0-4762-9F33-A5D2F8045B5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5229D150-52BC-47AD-BD06-C2E45FA28960}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15540" yWindow="3240" windowWidth="27810" windowHeight="16635" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5580" yWindow="4905" windowWidth="22800" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="5" sheetId="4" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="92">
   <si>
     <t>Bench</t>
   </si>
@@ -308,6 +308,15 @@
   </si>
   <si>
     <t>BV27(93)</t>
+  </si>
+  <si>
+    <t>HC6(11)</t>
+  </si>
+  <si>
+    <t>HC6(13)</t>
+  </si>
+  <si>
+    <t>HC6(15)</t>
   </si>
 </sst>
 </file>
@@ -631,10 +640,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6991F49-6444-43CA-9AF8-AA5E2FA14897}">
-  <dimension ref="A1:W17"/>
+  <dimension ref="A1:W20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="S6" sqref="S6:T6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M25" sqref="M25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -852,22 +861,22 @@
         <v>12</v>
       </c>
       <c r="S3">
-        <f t="shared" ref="S3:S17" si="3">(O3-Q3)/N3</f>
+        <f t="shared" ref="S3:S21" si="3">(O3-Q3)/N3</f>
         <v>0.2857142857142857</v>
       </c>
       <c r="T3">
-        <f t="shared" ref="T3:T17" si="4">(P3-R3+Q3)/N3</f>
+        <f t="shared" ref="T3:T21" si="4">(P3-R3+Q3)/N3</f>
         <v>0.2857142857142857</v>
       </c>
       <c r="U3">
-        <f t="shared" ref="U3:U17" si="5" xml:space="preserve"> 1 -R3/N3</f>
+        <f t="shared" ref="U3:U21" si="5" xml:space="preserve"> 1 -R3/N3</f>
         <v>0.5714285714285714</v>
       </c>
       <c r="V3">
         <v>0</v>
       </c>
       <c r="W3">
-        <f t="shared" ref="W3:W17" si="6">V3/N3</f>
+        <f t="shared" ref="W3:W21" si="6">V3/N3</f>
         <v>0</v>
       </c>
     </row>
@@ -1154,7 +1163,7 @@
         <v>16</v>
       </c>
       <c r="P7">
-        <f t="shared" ref="P7:P17" si="9">N7-O7</f>
+        <f t="shared" ref="P7:P21" si="9">N7-O7</f>
         <v>6</v>
       </c>
       <c r="Q7">
@@ -1813,6 +1822,126 @@
       <c r="W17">
         <f t="shared" si="6"/>
         <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="13:23" x14ac:dyDescent="0.25">
+      <c r="M18" t="s">
+        <v>91</v>
+      </c>
+      <c r="N18">
+        <v>32</v>
+      </c>
+      <c r="O18">
+        <v>18</v>
+      </c>
+      <c r="P18">
+        <f>N18-O18</f>
+        <v>14</v>
+      </c>
+      <c r="Q18">
+        <v>14</v>
+      </c>
+      <c r="R18">
+        <v>20</v>
+      </c>
+      <c r="S18">
+        <f>(O18-Q18)/N18</f>
+        <v>0.125</v>
+      </c>
+      <c r="T18">
+        <f>(P18-R18+Q18)/N18</f>
+        <v>0.25</v>
+      </c>
+      <c r="U18">
+        <f xml:space="preserve"> 1 -R18/N18</f>
+        <v>0.375</v>
+      </c>
+      <c r="V18">
+        <v>1</v>
+      </c>
+      <c r="W18">
+        <f>V18/N18</f>
+        <v>3.125E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="13:23" x14ac:dyDescent="0.25">
+      <c r="M19" t="s">
+        <v>90</v>
+      </c>
+      <c r="N19">
+        <v>32</v>
+      </c>
+      <c r="O19">
+        <v>18</v>
+      </c>
+      <c r="P19">
+        <f>N19-O19</f>
+        <v>14</v>
+      </c>
+      <c r="Q19">
+        <v>15</v>
+      </c>
+      <c r="R19">
+        <v>21</v>
+      </c>
+      <c r="S19">
+        <f>(O19-Q19)/N19</f>
+        <v>9.375E-2</v>
+      </c>
+      <c r="T19">
+        <f>(P19-R19+Q19)/N19</f>
+        <v>0.25</v>
+      </c>
+      <c r="U19">
+        <f xml:space="preserve"> 1 -R19/N19</f>
+        <v>0.34375</v>
+      </c>
+      <c r="V19">
+        <v>0</v>
+      </c>
+      <c r="W19">
+        <f>V19/N19</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="13:23" x14ac:dyDescent="0.25">
+      <c r="M20" t="s">
+        <v>89</v>
+      </c>
+      <c r="N20">
+        <v>32</v>
+      </c>
+      <c r="O20">
+        <v>18</v>
+      </c>
+      <c r="P20">
+        <f>N20-O20</f>
+        <v>14</v>
+      </c>
+      <c r="Q20">
+        <v>18</v>
+      </c>
+      <c r="R20">
+        <v>26</v>
+      </c>
+      <c r="S20">
+        <f>(O20-Q20)/N20</f>
+        <v>0</v>
+      </c>
+      <c r="T20">
+        <f>(P20-R20+Q20)/N20</f>
+        <v>0.1875</v>
+      </c>
+      <c r="U20">
+        <f xml:space="preserve"> 1 -R20/N20</f>
+        <v>0.1875</v>
+      </c>
+      <c r="V20">
+        <v>1</v>
+      </c>
+      <c r="W20">
+        <f>V20/N20</f>
+        <v>3.125E-2</v>
       </c>
     </row>
   </sheetData>
@@ -5126,7 +5255,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54E03DA5-84A0-4738-955A-CBE7B8794599}">
   <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>

</xml_diff>